<commit_message>
alter notebook dataframe order by values
</commit_message>
<xml_diff>
--- a/experiments/experiment_2/notebooks/estrategias.xlsx
+++ b/experiments/experiment_2/notebooks/estrategias.xlsx
@@ -16,25 +16,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>S1</t>
+    <t>Search</t>
   </si>
   <si>
-    <t>S2</t>
+    <t>Search + SB</t>
   </si>
   <si>
-    <t>S3</t>
+    <t>GS + SB</t>
   </si>
   <si>
-    <t>S4</t>
+    <t>Scopus + SB</t>
   </si>
   <si>
-    <t>S5</t>
+    <t>Scopus + BW // FW</t>
   </si>
   <si>
-    <t>S6</t>
+    <t>Scopus + BW + FW</t>
   </si>
   <si>
-    <t>S7</t>
+    <t>Scopus + FW + BW</t>
   </si>
 </sst>
 </file>

</xml_diff>